<commit_message>
functions for weekly, monthly and payrolls
</commit_message>
<xml_diff>
--- a/Generated files/replicated_format.xlsx
+++ b/Generated files/replicated_format.xlsx
@@ -1137,33 +1137,19 @@
       <c r="E4" t="n">
         <v>4</v>
       </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
-      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
         <v>4</v>
       </c>
       <c r="J4" t="n">
         <v>4.1</v>
       </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
       <c r="O4" t="n">
         <v>8</v>
       </c>
@@ -1182,30 +1168,18 @@
       <c r="T4" t="n">
         <v>3.93</v>
       </c>
-      <c r="U4" t="n">
-        <v>0</v>
-      </c>
-      <c r="V4" t="n">
-        <v>0</v>
-      </c>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
       <c r="W4" t="n">
         <v>4</v>
       </c>
       <c r="X4" t="n">
         <v>4.13</v>
       </c>
-      <c r="Y4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
       <c r="AC4" t="n">
         <v>8</v>
       </c>
@@ -1243,18 +1217,10 @@
           <t>Adriana Orellana</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
         <v>12</v>
       </c>
@@ -1267,36 +1233,20 @@
       <c r="J5" t="n">
         <v>12.52</v>
       </c>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="n">
         <v>10.4</v>
       </c>
       <c r="M5" t="n">
         <v>12</v>
       </c>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0</v>
-      </c>
-      <c r="T5" t="n">
-        <v>0</v>
-      </c>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
       <c r="U5" t="n">
         <v>12</v>
       </c>
@@ -1315,18 +1265,10 @@
       <c r="Z5" t="n">
         <v>10.52</v>
       </c>
-      <c r="AA5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>0</v>
-      </c>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
       <c r="AE5" t="n">
         <v>0</v>
       </c>
@@ -1358,90 +1300,54 @@
           <t>Anuj Kumar Singh Malik</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
         <v>6.77</v>
       </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
+      <c r="I6" t="inlineStr"/>
       <c r="J6" t="n">
         <v>8.529999999999999</v>
       </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="n">
         <v>8.880000000000001</v>
       </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
+      <c r="M6" t="inlineStr"/>
       <c r="N6" t="n">
         <v>7.03</v>
       </c>
-      <c r="O6" t="n">
-        <v>0</v>
-      </c>
+      <c r="O6" t="inlineStr"/>
       <c r="P6" t="n">
         <v>3.6</v>
       </c>
-      <c r="Q6" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q6" t="inlineStr"/>
       <c r="R6" t="n">
         <v>2.33</v>
       </c>
-      <c r="S6" t="n">
-        <v>0</v>
-      </c>
+      <c r="S6" t="inlineStr"/>
       <c r="T6" t="n">
         <v>8.5</v>
       </c>
-      <c r="U6" t="n">
-        <v>0</v>
-      </c>
+      <c r="U6" t="inlineStr"/>
       <c r="V6" t="n">
         <v>5.53</v>
       </c>
-      <c r="W6" t="n">
-        <v>0</v>
-      </c>
+      <c r="W6" t="inlineStr"/>
       <c r="X6" t="n">
         <v>7.95</v>
       </c>
-      <c r="Y6" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y6" t="inlineStr"/>
       <c r="Z6" t="n">
         <v>8.529999999999999</v>
       </c>
-      <c r="AA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>0</v>
-      </c>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
       <c r="AE6" t="n">
         <v>0</v>
       </c>
@@ -1473,90 +1379,54 @@
           <t>Brendaline Nettey</t>
         </is>
       </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
         <v>8.779999999999999</v>
       </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
         <v>8.68</v>
       </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="n">
         <v>8.699999999999999</v>
       </c>
-      <c r="K7" t="n">
-        <v>0</v>
-      </c>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="n">
         <v>8.449999999999999</v>
       </c>
-      <c r="M7" t="n">
-        <v>0</v>
-      </c>
+      <c r="M7" t="inlineStr"/>
       <c r="N7" t="n">
         <v>5.77</v>
       </c>
-      <c r="O7" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" t="n">
-        <v>0</v>
-      </c>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
       <c r="T7" t="n">
         <v>8.5</v>
       </c>
-      <c r="U7" t="n">
-        <v>0</v>
-      </c>
+      <c r="U7" t="inlineStr"/>
       <c r="V7" t="n">
         <v>8.630000000000001</v>
       </c>
-      <c r="W7" t="n">
-        <v>0</v>
-      </c>
+      <c r="W7" t="inlineStr"/>
       <c r="X7" t="n">
         <v>8.67</v>
       </c>
-      <c r="Y7" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="n">
         <v>8.58</v>
       </c>
-      <c r="AA7" t="n">
-        <v>0</v>
-      </c>
+      <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="n">
         <v>5.32</v>
       </c>
-      <c r="AC7" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC7" t="inlineStr"/>
+      <c r="AD7" t="inlineStr"/>
       <c r="AE7" t="n">
         <v>0</v>
       </c>
@@ -1588,12 +1458,8 @@
           <t>CLAUDIA CANAS</t>
         </is>
       </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="n">
         <v>6</v>
       </c>
@@ -1606,12 +1472,8 @@
       <c r="H8" t="n">
         <v>5.15</v>
       </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
       <c r="K8" t="n">
         <v>6</v>
       </c>
@@ -1624,36 +1486,22 @@
       <c r="N8" t="n">
         <v>5.12</v>
       </c>
-      <c r="O8" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" t="n">
-        <v>0</v>
-      </c>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
       <c r="S8" t="n">
         <v>6</v>
       </c>
-      <c r="T8" t="n">
-        <v>0</v>
-      </c>
+      <c r="T8" t="inlineStr"/>
       <c r="U8" t="n">
         <v>6</v>
       </c>
       <c r="V8" t="n">
         <v>5.45</v>
       </c>
-      <c r="W8" t="n">
-        <v>0</v>
-      </c>
-      <c r="X8" t="n">
-        <v>0</v>
-      </c>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
       <c r="Y8" t="n">
         <v>6</v>
       </c>
@@ -1666,12 +1514,8 @@
       <c r="AB8" t="n">
         <v>5.05</v>
       </c>
-      <c r="AC8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC8" t="inlineStr"/>
+      <c r="AD8" t="inlineStr"/>
       <c r="AE8" t="n">
         <v>0</v>
       </c>
@@ -1703,90 +1547,38 @@
           <t>Carol Cordrey</t>
         </is>
       </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0</v>
-      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
       <c r="Q9" t="n">
         <v>8</v>
       </c>
       <c r="R9" t="n">
         <v>8.1</v>
       </c>
-      <c r="S9" t="n">
-        <v>0</v>
-      </c>
-      <c r="T9" t="n">
-        <v>0</v>
-      </c>
-      <c r="U9" t="n">
-        <v>0</v>
-      </c>
-      <c r="V9" t="n">
-        <v>0</v>
-      </c>
-      <c r="W9" t="n">
-        <v>0</v>
-      </c>
-      <c r="X9" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y9" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC9" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD9" t="n">
-        <v>0</v>
-      </c>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
+      <c r="AB9" t="inlineStr"/>
+      <c r="AC9" t="inlineStr"/>
+      <c r="AD9" t="inlineStr"/>
       <c r="AE9" t="n">
         <v>0</v>
       </c>
@@ -1818,90 +1610,56 @@
           <t>Chisom Mgbodile</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
+      <c r="C10" t="inlineStr"/>
       <c r="D10" t="n">
         <v>8.470000000000001</v>
       </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
         <v>6.68</v>
       </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
+      <c r="I10" t="inlineStr"/>
       <c r="J10" t="n">
         <v>6.13</v>
       </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
+      <c r="K10" t="inlineStr"/>
       <c r="L10" t="n">
         <v>5.5</v>
       </c>
-      <c r="M10" t="n">
-        <v>0</v>
-      </c>
+      <c r="M10" t="inlineStr"/>
       <c r="N10" t="n">
         <v>7.13</v>
       </c>
-      <c r="O10" t="n">
-        <v>0</v>
-      </c>
+      <c r="O10" t="inlineStr"/>
       <c r="P10" t="n">
         <v>0.1</v>
       </c>
-      <c r="Q10" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q10" t="inlineStr"/>
       <c r="R10" t="n">
         <v>5.58</v>
       </c>
-      <c r="S10" t="n">
-        <v>0</v>
-      </c>
+      <c r="S10" t="inlineStr"/>
       <c r="T10" t="n">
         <v>7.37</v>
       </c>
-      <c r="U10" t="n">
-        <v>0</v>
-      </c>
+      <c r="U10" t="inlineStr"/>
       <c r="V10" t="n">
         <v>4.53</v>
       </c>
-      <c r="W10" t="n">
-        <v>0</v>
-      </c>
+      <c r="W10" t="inlineStr"/>
       <c r="X10" t="n">
         <v>6.87</v>
       </c>
-      <c r="Y10" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="n">
         <v>8.800000000000001</v>
       </c>
-      <c r="AA10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC10" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD10" t="n">
-        <v>0</v>
-      </c>
+      <c r="AA10" t="inlineStr"/>
+      <c r="AB10" t="inlineStr"/>
+      <c r="AC10" t="inlineStr"/>
+      <c r="AD10" t="inlineStr"/>
       <c r="AE10" t="n">
         <v>0</v>
       </c>
@@ -1933,12 +1691,8 @@
           <t>DIANA CANAS</t>
         </is>
       </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="n">
         <v>8</v>
       </c>
@@ -1969,18 +1723,10 @@
       <c r="N11" t="n">
         <v>12.22</v>
       </c>
-      <c r="O11" t="n">
-        <v>0</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>0</v>
-      </c>
-      <c r="R11" t="n">
-        <v>0</v>
-      </c>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
+      <c r="R11" t="inlineStr"/>
       <c r="S11" t="n">
         <v>8</v>
       </c>
@@ -2011,12 +1757,8 @@
       <c r="AB11" t="n">
         <v>12.15</v>
       </c>
-      <c r="AC11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD11" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC11" t="inlineStr"/>
+      <c r="AD11" t="inlineStr"/>
       <c r="AE11" t="n">
         <v>0</v>
       </c>
@@ -2048,12 +1790,8 @@
           <t>Dekonti Sayeh</t>
         </is>
       </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
         <v>12</v>
       </c>
@@ -2063,63 +1801,37 @@
       <c r="G12" t="n">
         <v>12</v>
       </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
       <c r="K12" t="n">
         <v>12</v>
       </c>
       <c r="L12" t="n">
         <v>12.08</v>
       </c>
-      <c r="M12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" t="n">
-        <v>0</v>
-      </c>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
+      <c r="R12" t="inlineStr"/>
       <c r="S12" t="n">
         <v>12</v>
       </c>
       <c r="T12" t="n">
         <v>12.12</v>
       </c>
-      <c r="U12" t="n">
-        <v>0</v>
-      </c>
-      <c r="V12" t="n">
-        <v>0</v>
-      </c>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
       <c r="W12" t="n">
         <v>12</v>
       </c>
       <c r="X12" t="n">
         <v>12.08</v>
       </c>
-      <c r="Y12" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z12" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y12" t="inlineStr"/>
+      <c r="Z12" t="inlineStr"/>
       <c r="AA12" t="n">
         <v>12</v>
       </c>
@@ -2163,90 +1875,54 @@
           <t>EDWARD CHAVEZ</t>
         </is>
       </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
         <v>8.27</v>
       </c>
-      <c r="G13" t="n">
-        <v>0</v>
-      </c>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="n">
         <v>8.550000000000001</v>
       </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
+      <c r="I13" t="inlineStr"/>
       <c r="J13" t="n">
         <v>8.1</v>
       </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
+      <c r="K13" t="inlineStr"/>
       <c r="L13" t="n">
         <v>7.95</v>
       </c>
-      <c r="M13" t="n">
-        <v>0</v>
-      </c>
+      <c r="M13" t="inlineStr"/>
       <c r="N13" t="n">
         <v>7.37</v>
       </c>
-      <c r="O13" t="n">
-        <v>0</v>
-      </c>
-      <c r="P13" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>0</v>
-      </c>
-      <c r="R13" t="n">
-        <v>0</v>
-      </c>
-      <c r="S13" t="n">
-        <v>0</v>
-      </c>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
       <c r="T13" t="n">
         <v>7.22</v>
       </c>
-      <c r="U13" t="n">
-        <v>0</v>
-      </c>
+      <c r="U13" t="inlineStr"/>
       <c r="V13" t="n">
         <v>8.119999999999999</v>
       </c>
-      <c r="W13" t="n">
-        <v>0</v>
-      </c>
+      <c r="W13" t="inlineStr"/>
       <c r="X13" t="n">
         <v>8.199999999999999</v>
       </c>
-      <c r="Y13" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y13" t="inlineStr"/>
       <c r="Z13" t="n">
         <v>8.92</v>
       </c>
-      <c r="AA13" t="n">
-        <v>0</v>
-      </c>
+      <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="n">
         <v>7.2</v>
       </c>
-      <c r="AC13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD13" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC13" t="inlineStr"/>
+      <c r="AD13" t="inlineStr"/>
       <c r="AE13" t="n">
         <v>0</v>
       </c>
@@ -2284,81 +1960,31 @@
       <c r="D14" t="n">
         <v>8.58</v>
       </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" t="n">
-        <v>0</v>
-      </c>
-      <c r="P14" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>0</v>
-      </c>
-      <c r="R14" t="n">
-        <v>0</v>
-      </c>
-      <c r="S14" t="n">
-        <v>0</v>
-      </c>
-      <c r="T14" t="n">
-        <v>0</v>
-      </c>
-      <c r="U14" t="n">
-        <v>0</v>
-      </c>
-      <c r="V14" t="n">
-        <v>0</v>
-      </c>
-      <c r="W14" t="n">
-        <v>0</v>
-      </c>
-      <c r="X14" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y14" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC14" t="n">
-        <v>0</v>
-      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
+      <c r="Z14" t="inlineStr"/>
+      <c r="AA14" t="inlineStr"/>
+      <c r="AB14" t="inlineStr"/>
+      <c r="AC14" t="inlineStr"/>
       <c r="AD14" t="n">
         <v>8.08</v>
       </c>
@@ -2393,90 +2019,56 @@
           <t>Francis Mgbodile</t>
         </is>
       </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="n">
         <v>6.43</v>
       </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0</v>
-      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
       <c r="H15" t="n">
         <v>6.5</v>
       </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="n">
         <v>6.88</v>
       </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
+      <c r="K15" t="inlineStr"/>
       <c r="L15" t="n">
         <v>5.38</v>
       </c>
-      <c r="M15" t="n">
-        <v>0</v>
-      </c>
+      <c r="M15" t="inlineStr"/>
       <c r="N15" t="n">
         <v>6.75</v>
       </c>
-      <c r="O15" t="n">
-        <v>0</v>
-      </c>
+      <c r="O15" t="inlineStr"/>
       <c r="P15" t="n">
         <v>2.52</v>
       </c>
-      <c r="Q15" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q15" t="inlineStr"/>
       <c r="R15" t="n">
         <v>3</v>
       </c>
-      <c r="S15" t="n">
-        <v>0</v>
-      </c>
+      <c r="S15" t="inlineStr"/>
       <c r="T15" t="n">
         <v>6.72</v>
       </c>
-      <c r="U15" t="n">
-        <v>0</v>
-      </c>
+      <c r="U15" t="inlineStr"/>
       <c r="V15" t="n">
         <v>4.55</v>
       </c>
-      <c r="W15" t="n">
-        <v>0</v>
-      </c>
+      <c r="W15" t="inlineStr"/>
       <c r="X15" t="n">
         <v>5.5</v>
       </c>
-      <c r="Y15" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y15" t="inlineStr"/>
       <c r="Z15" t="n">
         <v>7.37</v>
       </c>
-      <c r="AA15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC15" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD15" t="n">
-        <v>0</v>
-      </c>
+      <c r="AA15" t="inlineStr"/>
+      <c r="AB15" t="inlineStr"/>
+      <c r="AC15" t="inlineStr"/>
+      <c r="AD15" t="inlineStr"/>
       <c r="AE15" t="n">
         <v>0</v>
       </c>
@@ -2508,78 +2100,46 @@
           <t>Grace Garbo</t>
         </is>
       </c>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
       <c r="E16" t="n">
         <v>4</v>
       </c>
       <c r="F16" t="n">
         <v>4.53</v>
       </c>
-      <c r="G16" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0</v>
-      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
       <c r="M16" t="n">
         <v>8.5</v>
       </c>
       <c r="N16" t="n">
         <v>4.85</v>
       </c>
-      <c r="O16" t="n">
-        <v>0</v>
-      </c>
-      <c r="P16" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>0</v>
-      </c>
-      <c r="R16" t="n">
-        <v>0</v>
-      </c>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
+      <c r="R16" t="inlineStr"/>
       <c r="S16" t="n">
         <v>4</v>
       </c>
       <c r="T16" t="n">
         <v>6.27</v>
       </c>
-      <c r="U16" t="n">
-        <v>0</v>
-      </c>
-      <c r="V16" t="n">
-        <v>0</v>
-      </c>
-      <c r="W16" t="n">
-        <v>0</v>
-      </c>
-      <c r="X16" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>0</v>
-      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>UL</t>
+        </is>
+      </c>
+      <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
+      <c r="X16" t="inlineStr"/>
+      <c r="Y16" t="inlineStr"/>
+      <c r="Z16" t="inlineStr"/>
       <c r="AA16" t="n">
         <v>8.5</v>
       </c>
@@ -2623,90 +2183,52 @@
           <t>Hiwot Mideksa</t>
         </is>
       </c>
-      <c r="C17" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0</v>
-      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr"/>
       <c r="H17" t="n">
         <v>7.15</v>
       </c>
-      <c r="I17" t="n">
-        <v>0</v>
-      </c>
+      <c r="I17" t="inlineStr"/>
       <c r="J17" t="n">
         <v>8.5</v>
       </c>
-      <c r="K17" t="n">
-        <v>0</v>
-      </c>
+      <c r="K17" t="inlineStr"/>
       <c r="L17" t="n">
         <v>8.529999999999999</v>
       </c>
-      <c r="M17" t="n">
-        <v>0</v>
-      </c>
+      <c r="M17" t="inlineStr"/>
       <c r="N17" t="n">
         <v>7.63</v>
       </c>
-      <c r="O17" t="n">
-        <v>0</v>
-      </c>
+      <c r="O17" t="inlineStr"/>
       <c r="P17" t="n">
         <v>8.35</v>
       </c>
-      <c r="Q17" t="n">
-        <v>0</v>
-      </c>
-      <c r="R17" t="n">
-        <v>0</v>
-      </c>
-      <c r="S17" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q17" t="inlineStr"/>
+      <c r="R17" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
       <c r="T17" t="n">
         <v>2.1</v>
       </c>
-      <c r="U17" t="n">
-        <v>0</v>
-      </c>
+      <c r="U17" t="inlineStr"/>
       <c r="V17" t="n">
         <v>8</v>
       </c>
-      <c r="W17" t="n">
-        <v>0</v>
-      </c>
+      <c r="W17" t="inlineStr"/>
       <c r="X17" t="n">
         <v>8.5</v>
       </c>
-      <c r="Y17" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y17" t="inlineStr"/>
       <c r="Z17" t="n">
         <v>8</v>
       </c>
-      <c r="AA17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD17" t="n">
-        <v>0</v>
-      </c>
+      <c r="AA17" t="inlineStr"/>
+      <c r="AB17" t="inlineStr"/>
+      <c r="AC17" t="inlineStr"/>
+      <c r="AD17" t="inlineStr"/>
       <c r="AE17" t="n">
         <v>0</v>
       </c>
@@ -2738,18 +2260,10 @@
           <t>JOSELUIS JIMENEZ</t>
         </is>
       </c>
-      <c r="C18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" t="n">
-        <v>0</v>
-      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr"/>
       <c r="G18" t="n">
         <v>11</v>
       </c>
@@ -2774,18 +2288,12 @@
       <c r="N18" t="n">
         <v>8</v>
       </c>
-      <c r="O18" t="n">
-        <v>0</v>
-      </c>
+      <c r="O18" t="inlineStr"/>
       <c r="P18" t="n">
         <v>3</v>
       </c>
-      <c r="Q18" t="n">
-        <v>0</v>
-      </c>
-      <c r="R18" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
       <c r="S18" t="n">
         <v>8</v>
       </c>
@@ -2853,12 +2361,8 @@
           <t>Jocelyn Andrade</t>
         </is>
       </c>
-      <c r="C19" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="n">
         <v>8.5</v>
       </c>
@@ -2889,18 +2393,10 @@
       <c r="N19" t="n">
         <v>8.02</v>
       </c>
-      <c r="O19" t="n">
-        <v>0</v>
-      </c>
-      <c r="P19" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>0</v>
-      </c>
-      <c r="R19" t="n">
-        <v>0</v>
-      </c>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
       <c r="S19" t="n">
         <v>8.5</v>
       </c>
@@ -2931,12 +2427,8 @@
       <c r="AB19" t="n">
         <v>7.53</v>
       </c>
-      <c r="AC19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD19" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC19" t="inlineStr"/>
+      <c r="AD19" t="inlineStr"/>
       <c r="AE19" t="n">
         <v>0</v>
       </c>
@@ -2968,12 +2460,8 @@
           <t>KAREN JIMENEZ</t>
         </is>
       </c>
-      <c r="C20" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="n">
         <v>10</v>
       </c>
@@ -2998,24 +2486,12 @@
       <c r="L20" t="n">
         <v>10</v>
       </c>
-      <c r="M20" t="n">
-        <v>0</v>
-      </c>
-      <c r="N20" t="n">
-        <v>0</v>
-      </c>
-      <c r="O20" t="n">
-        <v>0</v>
-      </c>
-      <c r="P20" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q20" t="n">
-        <v>0</v>
-      </c>
-      <c r="R20" t="n">
-        <v>0</v>
-      </c>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
       <c r="S20" t="n">
         <v>10</v>
       </c>
@@ -3028,9 +2504,7 @@
       <c r="V20" t="n">
         <v>9.949999999999999</v>
       </c>
-      <c r="W20" t="n">
-        <v>0</v>
-      </c>
+      <c r="W20" t="inlineStr"/>
       <c r="X20" t="n">
         <v>8.65</v>
       </c>
@@ -3040,12 +2514,8 @@
       <c r="Z20" t="n">
         <v>9.4</v>
       </c>
-      <c r="AA20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB20" t="n">
-        <v>0</v>
-      </c>
+      <c r="AA20" t="inlineStr"/>
+      <c r="AB20" t="inlineStr"/>
       <c r="AC20" t="n">
         <v>6</v>
       </c>
@@ -3083,12 +2553,8 @@
           <t>Keanna Wood</t>
         </is>
       </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="n">
         <v>8.5</v>
       </c>
@@ -3104,33 +2570,21 @@
       <c r="I21" t="n">
         <v>8.5</v>
       </c>
-      <c r="J21" t="n">
-        <v>0</v>
-      </c>
+      <c r="J21" t="inlineStr"/>
       <c r="K21" t="n">
         <v>8.5</v>
       </c>
-      <c r="L21" t="n">
-        <v>0</v>
-      </c>
+      <c r="L21" t="inlineStr"/>
       <c r="M21" t="n">
         <v>8.5</v>
       </c>
       <c r="N21" t="n">
         <v>8.08</v>
       </c>
-      <c r="O21" t="n">
-        <v>0</v>
-      </c>
-      <c r="P21" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>0</v>
-      </c>
-      <c r="R21" t="n">
-        <v>0</v>
-      </c>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
       <c r="S21" t="n">
         <v>8.5</v>
       </c>
@@ -3146,9 +2600,7 @@
       <c r="W21" t="n">
         <v>8.5</v>
       </c>
-      <c r="X21" t="n">
-        <v>0</v>
-      </c>
+      <c r="X21" t="inlineStr"/>
       <c r="Y21" t="n">
         <v>8.5</v>
       </c>
@@ -3161,12 +2613,8 @@
       <c r="AB21" t="n">
         <v>8.050000000000001</v>
       </c>
-      <c r="AC21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD21" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC21" t="inlineStr"/>
+      <c r="AD21" t="inlineStr"/>
       <c r="AE21" t="n">
         <v>0</v>
       </c>
@@ -3198,90 +2646,52 @@
           <t>LAURYN CRAWLEY</t>
         </is>
       </c>
-      <c r="C22" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
         <v>6.95</v>
       </c>
-      <c r="G22" t="n">
-        <v>0</v>
-      </c>
+      <c r="G22" t="inlineStr"/>
       <c r="H22" t="n">
         <v>5.93</v>
       </c>
-      <c r="I22" t="n">
-        <v>0</v>
-      </c>
-      <c r="J22" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" t="n">
-        <v>0</v>
-      </c>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
       <c r="L22" t="n">
         <v>3.63</v>
       </c>
-      <c r="M22" t="n">
-        <v>0</v>
-      </c>
+      <c r="M22" t="inlineStr"/>
       <c r="N22" t="n">
         <v>3.52</v>
       </c>
-      <c r="O22" t="n">
-        <v>0</v>
-      </c>
-      <c r="P22" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>0</v>
-      </c>
-      <c r="R22" t="n">
-        <v>0</v>
-      </c>
-      <c r="S22" t="n">
-        <v>0</v>
-      </c>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
       <c r="T22" t="n">
         <v>1.8</v>
       </c>
-      <c r="U22" t="n">
-        <v>0</v>
-      </c>
+      <c r="U22" t="inlineStr"/>
       <c r="V22" t="n">
         <v>5.67</v>
       </c>
-      <c r="W22" t="n">
-        <v>0</v>
-      </c>
+      <c r="W22" t="inlineStr"/>
       <c r="X22" t="n">
         <v>5.07</v>
       </c>
-      <c r="Y22" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y22" t="inlineStr"/>
       <c r="Z22" t="n">
         <v>5</v>
       </c>
-      <c r="AA22" t="n">
-        <v>0</v>
-      </c>
+      <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="n">
         <v>2.6</v>
       </c>
-      <c r="AC22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD22" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC22" t="inlineStr"/>
+      <c r="AD22" t="inlineStr"/>
       <c r="AE22" t="n">
         <v>0</v>
       </c>
@@ -3313,12 +2723,8 @@
           <t>LEONARD KASSIS</t>
         </is>
       </c>
-      <c r="C23" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0</v>
-      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="n">
         <v>8.5</v>
       </c>
@@ -3349,20 +2755,14 @@
       <c r="N23" t="n">
         <v>8</v>
       </c>
-      <c r="O23" t="n">
-        <v>0</v>
-      </c>
-      <c r="P23" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q23" t="n">
-        <v>0</v>
-      </c>
-      <c r="R23" t="n">
-        <v>0</v>
-      </c>
-      <c r="S23" t="n">
-        <v>0</v>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>PTO</t>
+        </is>
       </c>
       <c r="T23" t="n">
         <v>8.25</v>
@@ -3385,18 +2785,16 @@
       <c r="Z23" t="n">
         <v>8.6</v>
       </c>
-      <c r="AA23" t="n">
-        <v>3.5</v>
+      <c r="AA23" t="inlineStr">
+        <is>
+          <t>PTO</t>
+        </is>
       </c>
       <c r="AB23" t="n">
         <v>3.7</v>
       </c>
-      <c r="AC23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD23" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC23" t="inlineStr"/>
+      <c r="AD23" t="inlineStr"/>
       <c r="AE23" t="n">
         <v>0</v>
       </c>
@@ -3416,7 +2814,7 @@
         <v>16.38</v>
       </c>
       <c r="AK23" t="n">
-        <v>20.5</v>
+        <v>17</v>
       </c>
       <c r="AL23" t="n">
         <v>20.48</v>
@@ -3428,12 +2826,8 @@
           <t>LILIANA HENRIQUEZ</t>
         </is>
       </c>
-      <c r="C24" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0</v>
-      </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="n">
         <v>8.75</v>
       </c>
@@ -3464,18 +2858,10 @@
       <c r="N24" t="n">
         <v>8.800000000000001</v>
       </c>
-      <c r="O24" t="n">
-        <v>0</v>
-      </c>
-      <c r="P24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>0</v>
-      </c>
-      <c r="R24" t="n">
-        <v>0</v>
-      </c>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
+      <c r="Q24" t="inlineStr"/>
+      <c r="R24" t="inlineStr"/>
       <c r="S24" t="n">
         <v>8.75</v>
       </c>
@@ -3506,12 +2892,8 @@
       <c r="AB24" t="n">
         <v>9.42</v>
       </c>
-      <c r="AC24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD24" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC24" t="inlineStr"/>
+      <c r="AD24" t="inlineStr"/>
       <c r="AE24" t="n">
         <v>0</v>
       </c>
@@ -3543,90 +2925,46 @@
           <t>MANBIR TAKHAR</t>
         </is>
       </c>
-      <c r="C25" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
         <v>8</v>
       </c>
-      <c r="F25" t="n">
-        <v>0</v>
-      </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="n">
         <v>8</v>
       </c>
-      <c r="H25" t="n">
-        <v>0</v>
-      </c>
-      <c r="I25" t="n">
-        <v>0</v>
-      </c>
-      <c r="J25" t="n">
-        <v>0</v>
-      </c>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
       <c r="K25" t="n">
         <v>8</v>
       </c>
-      <c r="L25" t="n">
-        <v>0</v>
-      </c>
-      <c r="M25" t="n">
-        <v>0</v>
-      </c>
-      <c r="N25" t="n">
-        <v>0</v>
-      </c>
-      <c r="O25" t="n">
-        <v>0</v>
-      </c>
-      <c r="P25" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>0</v>
-      </c>
-      <c r="R25" t="n">
-        <v>0</v>
-      </c>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
+      <c r="Q25" t="inlineStr"/>
+      <c r="R25" t="inlineStr"/>
       <c r="S25" t="n">
         <v>8</v>
       </c>
-      <c r="T25" t="n">
-        <v>0</v>
-      </c>
+      <c r="T25" t="inlineStr"/>
       <c r="U25" t="n">
         <v>8</v>
       </c>
-      <c r="V25" t="n">
-        <v>0</v>
-      </c>
-      <c r="W25" t="n">
-        <v>0</v>
-      </c>
-      <c r="X25" t="n">
-        <v>0</v>
-      </c>
+      <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr"/>
+      <c r="X25" t="inlineStr"/>
       <c r="Y25" t="n">
         <v>8</v>
       </c>
-      <c r="Z25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD25" t="n">
-        <v>0</v>
-      </c>
+      <c r="Z25" t="inlineStr"/>
+      <c r="AA25" t="inlineStr"/>
+      <c r="AB25" t="inlineStr"/>
+      <c r="AC25" t="inlineStr"/>
+      <c r="AD25" t="inlineStr"/>
       <c r="AE25" t="n">
         <v>0</v>
       </c>
@@ -3658,84 +2996,32 @@
           <t>MARIADAN GONZALEZ VASQUEZ</t>
         </is>
       </c>
-      <c r="C26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0</v>
-      </c>
-      <c r="I26" t="n">
-        <v>0</v>
-      </c>
-      <c r="J26" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" t="n">
-        <v>0</v>
-      </c>
-      <c r="L26" t="n">
-        <v>0</v>
-      </c>
-      <c r="M26" t="n">
-        <v>0</v>
-      </c>
-      <c r="N26" t="n">
-        <v>0</v>
-      </c>
-      <c r="O26" t="n">
-        <v>0</v>
-      </c>
-      <c r="P26" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q26" t="n">
-        <v>0</v>
-      </c>
-      <c r="R26" t="n">
-        <v>0</v>
-      </c>
-      <c r="S26" t="n">
-        <v>0</v>
-      </c>
-      <c r="T26" t="n">
-        <v>0</v>
-      </c>
-      <c r="U26" t="n">
-        <v>0</v>
-      </c>
-      <c r="V26" t="n">
-        <v>0</v>
-      </c>
-      <c r="W26" t="n">
-        <v>0</v>
-      </c>
-      <c r="X26" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y26" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB26" t="n">
-        <v>0</v>
-      </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="inlineStr"/>
+      <c r="T26" t="inlineStr"/>
+      <c r="U26" t="inlineStr"/>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="inlineStr"/>
+      <c r="X26" t="inlineStr"/>
+      <c r="Y26" t="inlineStr"/>
+      <c r="Z26" t="inlineStr"/>
+      <c r="AA26" t="inlineStr"/>
+      <c r="AB26" t="inlineStr"/>
       <c r="AC26" t="n">
         <v>7</v>
       </c>
@@ -3779,84 +3065,50 @@
       <c r="D27" t="n">
         <v>7.75</v>
       </c>
-      <c r="E27" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" t="n">
-        <v>0</v>
-      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
       <c r="G27" t="n">
         <v>8</v>
       </c>
       <c r="H27" t="n">
         <v>8.630000000000001</v>
       </c>
-      <c r="I27" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" t="n">
-        <v>0</v>
-      </c>
-      <c r="L27" t="n">
-        <v>0</v>
-      </c>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
       <c r="M27" t="n">
         <v>12</v>
       </c>
       <c r="N27" t="n">
         <v>12.53</v>
       </c>
-      <c r="O27" t="n">
-        <v>0</v>
-      </c>
-      <c r="P27" t="n">
-        <v>0</v>
-      </c>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
       <c r="Q27" t="n">
         <v>8</v>
       </c>
-      <c r="R27" t="n">
-        <v>0</v>
-      </c>
-      <c r="S27" t="n">
-        <v>0</v>
-      </c>
-      <c r="T27" t="n">
-        <v>0</v>
-      </c>
+      <c r="R27" t="inlineStr"/>
+      <c r="S27" t="inlineStr"/>
+      <c r="T27" t="inlineStr"/>
       <c r="U27" t="n">
         <v>8</v>
       </c>
       <c r="V27" t="n">
         <v>8.25</v>
       </c>
-      <c r="W27" t="n">
-        <v>0</v>
-      </c>
-      <c r="X27" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y27" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z27" t="n">
-        <v>0</v>
-      </c>
+      <c r="W27" t="inlineStr"/>
+      <c r="X27" t="inlineStr"/>
+      <c r="Y27" t="inlineStr"/>
+      <c r="Z27" t="inlineStr"/>
       <c r="AA27" t="n">
         <v>12</v>
       </c>
       <c r="AB27" t="n">
         <v>9.529999999999999</v>
       </c>
-      <c r="AC27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD27" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC27" t="inlineStr"/>
+      <c r="AD27" t="inlineStr"/>
       <c r="AE27" t="n">
         <v>8</v>
       </c>
@@ -3888,12 +3140,8 @@
           <t>MELANIE QUEZADA LOPEZ</t>
         </is>
       </c>
-      <c r="C28" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" t="n">
-        <v>0</v>
-      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
       <c r="E28" t="n">
         <v>8.75</v>
       </c>
@@ -3924,18 +3172,10 @@
       <c r="N28" t="n">
         <v>7.97</v>
       </c>
-      <c r="O28" t="n">
-        <v>0</v>
-      </c>
-      <c r="P28" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R28" t="n">
-        <v>0</v>
-      </c>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="inlineStr"/>
       <c r="S28" t="n">
         <v>8.75</v>
       </c>
@@ -3966,12 +3206,8 @@
       <c r="AB28" t="n">
         <v>7.82</v>
       </c>
-      <c r="AC28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD28" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC28" t="inlineStr"/>
+      <c r="AD28" t="inlineStr"/>
       <c r="AE28" t="n">
         <v>0</v>
       </c>
@@ -4003,90 +3239,42 @@
           <t>Mahashweta Ghosh</t>
         </is>
       </c>
-      <c r="C29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" t="n">
-        <v>0</v>
-      </c>
-      <c r="G29" t="n">
-        <v>0</v>
-      </c>
-      <c r="H29" t="n">
-        <v>0</v>
-      </c>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr"/>
+      <c r="H29" t="inlineStr"/>
       <c r="I29" t="n">
         <v>6</v>
       </c>
-      <c r="J29" t="n">
-        <v>0</v>
-      </c>
-      <c r="K29" t="n">
-        <v>0</v>
-      </c>
-      <c r="L29" t="n">
-        <v>0</v>
-      </c>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
       <c r="M29" t="n">
         <v>6</v>
       </c>
-      <c r="N29" t="n">
-        <v>0</v>
-      </c>
-      <c r="O29" t="n">
-        <v>0</v>
-      </c>
-      <c r="P29" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q29" t="n">
-        <v>0</v>
-      </c>
-      <c r="R29" t="n">
-        <v>0</v>
-      </c>
-      <c r="S29" t="n">
-        <v>0</v>
-      </c>
-      <c r="T29" t="n">
-        <v>0</v>
-      </c>
-      <c r="U29" t="n">
-        <v>0</v>
-      </c>
-      <c r="V29" t="n">
-        <v>0</v>
-      </c>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
+      <c r="Q29" t="inlineStr"/>
+      <c r="R29" t="inlineStr"/>
+      <c r="S29" t="inlineStr"/>
+      <c r="T29" t="inlineStr"/>
+      <c r="U29" t="inlineStr"/>
+      <c r="V29" t="inlineStr"/>
       <c r="W29" t="n">
         <v>6</v>
       </c>
-      <c r="X29" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y29" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z29" t="n">
-        <v>0</v>
-      </c>
+      <c r="X29" t="inlineStr"/>
+      <c r="Y29" t="inlineStr"/>
+      <c r="Z29" t="inlineStr"/>
       <c r="AA29" t="n">
         <v>6</v>
       </c>
-      <c r="AB29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD29" t="n">
-        <v>0</v>
-      </c>
+      <c r="AB29" t="inlineStr"/>
+      <c r="AC29" t="inlineStr"/>
+      <c r="AD29" t="inlineStr"/>
       <c r="AE29" t="n">
         <v>0</v>
       </c>
@@ -4118,21 +3306,11 @@
           <t>Maria Wingo</t>
         </is>
       </c>
-      <c r="C30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" t="n">
-        <v>0</v>
-      </c>
-      <c r="G30" t="n">
-        <v>0</v>
-      </c>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr"/>
       <c r="H30" t="n">
         <v>3.65</v>
       </c>
@@ -4142,66 +3320,38 @@
       <c r="J30" t="n">
         <v>6.27</v>
       </c>
-      <c r="K30" t="n">
-        <v>0</v>
-      </c>
-      <c r="L30" t="n">
-        <v>0</v>
-      </c>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
       <c r="M30" t="n">
         <v>7</v>
       </c>
       <c r="N30" t="n">
         <v>5.97</v>
       </c>
-      <c r="O30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P30" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q30" t="n">
-        <v>0</v>
-      </c>
-      <c r="R30" t="n">
-        <v>0</v>
-      </c>
-      <c r="S30" t="n">
-        <v>0</v>
-      </c>
-      <c r="T30" t="n">
-        <v>0</v>
-      </c>
-      <c r="U30" t="n">
-        <v>0</v>
-      </c>
-      <c r="V30" t="n">
-        <v>0</v>
-      </c>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
+      <c r="Q30" t="inlineStr"/>
+      <c r="R30" t="inlineStr"/>
+      <c r="S30" t="inlineStr"/>
+      <c r="T30" t="inlineStr"/>
+      <c r="U30" t="inlineStr"/>
+      <c r="V30" t="inlineStr"/>
       <c r="W30" t="n">
         <v>7</v>
       </c>
       <c r="X30" t="n">
         <v>6.4</v>
       </c>
-      <c r="Y30" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z30" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y30" t="inlineStr"/>
+      <c r="Z30" t="inlineStr"/>
       <c r="AA30" t="n">
         <v>7</v>
       </c>
       <c r="AB30" t="n">
         <v>5.25</v>
       </c>
-      <c r="AC30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD30" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC30" t="inlineStr"/>
+      <c r="AD30" t="inlineStr"/>
       <c r="AE30" t="n">
         <v>0</v>
       </c>
@@ -4239,84 +3389,36 @@
       <c r="D31" t="n">
         <v>8.550000000000001</v>
       </c>
-      <c r="E31" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" t="n">
-        <v>0</v>
-      </c>
-      <c r="G31" t="n">
-        <v>0</v>
-      </c>
-      <c r="H31" t="n">
-        <v>0</v>
-      </c>
-      <c r="I31" t="n">
-        <v>0</v>
-      </c>
-      <c r="J31" t="n">
-        <v>0</v>
-      </c>
-      <c r="K31" t="n">
-        <v>0</v>
-      </c>
-      <c r="L31" t="n">
-        <v>0</v>
-      </c>
-      <c r="M31" t="n">
-        <v>0</v>
-      </c>
-      <c r="N31" t="n">
-        <v>0</v>
-      </c>
-      <c r="O31" t="n">
-        <v>0</v>
-      </c>
-      <c r="P31" t="n">
-        <v>0</v>
-      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
       <c r="Q31" t="n">
         <v>8</v>
       </c>
       <c r="R31" t="n">
         <v>8.67</v>
       </c>
-      <c r="S31" t="n">
-        <v>0</v>
-      </c>
-      <c r="T31" t="n">
-        <v>0</v>
-      </c>
-      <c r="U31" t="n">
-        <v>0</v>
-      </c>
-      <c r="V31" t="n">
-        <v>0</v>
-      </c>
-      <c r="W31" t="n">
-        <v>0</v>
-      </c>
-      <c r="X31" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y31" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD31" t="n">
-        <v>0</v>
-      </c>
+      <c r="S31" t="inlineStr"/>
+      <c r="T31" t="inlineStr"/>
+      <c r="U31" t="inlineStr"/>
+      <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr"/>
+      <c r="X31" t="inlineStr"/>
+      <c r="Y31" t="inlineStr"/>
+      <c r="Z31" t="inlineStr"/>
+      <c r="AA31" t="inlineStr"/>
+      <c r="AB31" t="inlineStr"/>
+      <c r="AC31" t="inlineStr"/>
+      <c r="AD31" t="inlineStr"/>
       <c r="AE31" t="n">
         <v>8</v>
       </c>
@@ -4348,12 +3450,8 @@
           <t>NEHALI PATEL</t>
         </is>
       </c>
-      <c r="C32" t="n">
-        <v>0</v>
-      </c>
-      <c r="D32" t="n">
-        <v>0</v>
-      </c>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
       <c r="E32" t="n">
         <v>9.5</v>
       </c>
@@ -4378,24 +3476,16 @@
       <c r="L32" t="n">
         <v>11.48</v>
       </c>
-      <c r="M32" t="n">
-        <v>0</v>
-      </c>
-      <c r="N32" t="n">
-        <v>0</v>
-      </c>
-      <c r="O32" t="n">
-        <v>0</v>
-      </c>
-      <c r="P32" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q32" t="n">
-        <v>0</v>
-      </c>
-      <c r="R32" t="n">
-        <v>0</v>
-      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>UL</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr"/>
+      <c r="R32" t="inlineStr"/>
       <c r="S32" t="n">
         <v>9.5</v>
       </c>
@@ -4426,12 +3516,8 @@
       <c r="AB32" t="n">
         <v>5.75</v>
       </c>
-      <c r="AC32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD32" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC32" t="inlineStr"/>
+      <c r="AD32" t="inlineStr"/>
       <c r="AE32" t="n">
         <v>0</v>
       </c>
@@ -4463,90 +3549,38 @@
           <t>NICOLE HICKSON</t>
         </is>
       </c>
-      <c r="C33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G33" t="n">
-        <v>0</v>
-      </c>
-      <c r="H33" t="n">
-        <v>0</v>
-      </c>
-      <c r="I33" t="n">
-        <v>0</v>
-      </c>
-      <c r="J33" t="n">
-        <v>0</v>
-      </c>
-      <c r="K33" t="n">
-        <v>0</v>
-      </c>
-      <c r="L33" t="n">
-        <v>0</v>
-      </c>
-      <c r="M33" t="n">
-        <v>0</v>
-      </c>
-      <c r="N33" t="n">
-        <v>0</v>
-      </c>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr"/>
       <c r="O33" t="n">
         <v>8</v>
       </c>
       <c r="P33" t="n">
         <v>7.05</v>
       </c>
-      <c r="Q33" t="n">
-        <v>0</v>
-      </c>
-      <c r="R33" t="n">
-        <v>0</v>
-      </c>
-      <c r="S33" t="n">
-        <v>0</v>
-      </c>
-      <c r="T33" t="n">
-        <v>0</v>
-      </c>
-      <c r="U33" t="n">
-        <v>0</v>
-      </c>
-      <c r="V33" t="n">
-        <v>0</v>
-      </c>
-      <c r="W33" t="n">
-        <v>0</v>
-      </c>
-      <c r="X33" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y33" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD33" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q33" t="inlineStr"/>
+      <c r="R33" t="inlineStr"/>
+      <c r="S33" t="inlineStr"/>
+      <c r="T33" t="inlineStr"/>
+      <c r="U33" t="inlineStr"/>
+      <c r="V33" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
+      <c r="X33" t="inlineStr"/>
+      <c r="Y33" t="inlineStr"/>
+      <c r="Z33" t="inlineStr"/>
+      <c r="AA33" t="inlineStr"/>
+      <c r="AB33" t="inlineStr"/>
+      <c r="AC33" t="inlineStr"/>
+      <c r="AD33" t="inlineStr"/>
       <c r="AE33" t="n">
         <v>0</v>
       </c>
@@ -4578,12 +3612,8 @@
           <t>NISHTHA SANGHANI</t>
         </is>
       </c>
-      <c r="C34" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0</v>
-      </c>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
       <c r="E34" t="n">
         <v>6</v>
       </c>
@@ -4596,9 +3626,7 @@
       <c r="H34" t="n">
         <v>7.23</v>
       </c>
-      <c r="I34" t="n">
-        <v>0</v>
-      </c>
+      <c r="I34" t="inlineStr"/>
       <c r="J34" t="n">
         <v>2.53</v>
       </c>
@@ -4614,18 +3642,12 @@
       <c r="N34" t="n">
         <v>8.470000000000001</v>
       </c>
-      <c r="O34" t="n">
-        <v>0</v>
-      </c>
+      <c r="O34" t="inlineStr"/>
       <c r="P34" t="n">
         <v>2.92</v>
       </c>
-      <c r="Q34" t="n">
-        <v>0</v>
-      </c>
-      <c r="R34" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q34" t="inlineStr"/>
+      <c r="R34" t="inlineStr"/>
       <c r="S34" t="n">
         <v>6</v>
       </c>
@@ -4638,12 +3660,8 @@
       <c r="V34" t="n">
         <v>9.73</v>
       </c>
-      <c r="W34" t="n">
-        <v>0</v>
-      </c>
-      <c r="X34" t="n">
-        <v>0</v>
-      </c>
+      <c r="W34" t="inlineStr"/>
+      <c r="X34" t="inlineStr"/>
       <c r="Y34" t="n">
         <v>6</v>
       </c>
@@ -4656,9 +3674,7 @@
       <c r="AB34" t="n">
         <v>6.93</v>
       </c>
-      <c r="AC34" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC34" t="inlineStr"/>
       <c r="AD34" t="n">
         <v>0.78</v>
       </c>
@@ -4693,87 +3709,51 @@
           <t>Naufin Ashraf</t>
         </is>
       </c>
-      <c r="C35" t="n">
-        <v>0</v>
-      </c>
+      <c r="C35" t="inlineStr"/>
       <c r="D35" t="n">
         <v>7.25</v>
       </c>
-      <c r="E35" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" t="n">
-        <v>0</v>
-      </c>
-      <c r="G35" t="n">
-        <v>0</v>
-      </c>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
       <c r="H35" t="n">
         <v>7.13</v>
       </c>
-      <c r="I35" t="n">
-        <v>0</v>
-      </c>
+      <c r="I35" t="inlineStr"/>
       <c r="J35" t="n">
         <v>10.43</v>
       </c>
-      <c r="K35" t="n">
-        <v>0</v>
-      </c>
+      <c r="K35" t="inlineStr"/>
       <c r="L35" t="n">
         <v>8.57</v>
       </c>
-      <c r="M35" t="n">
-        <v>0</v>
-      </c>
-      <c r="N35" t="n">
-        <v>0</v>
-      </c>
-      <c r="O35" t="n">
-        <v>0</v>
-      </c>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr"/>
+      <c r="O35" t="inlineStr"/>
       <c r="P35" t="n">
         <v>7.9</v>
       </c>
-      <c r="Q35" t="n">
-        <v>0</v>
-      </c>
-      <c r="R35" t="n">
-        <v>0</v>
-      </c>
-      <c r="S35" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q35" t="inlineStr"/>
+      <c r="R35" t="inlineStr"/>
+      <c r="S35" t="inlineStr"/>
       <c r="T35" t="n">
         <v>9.27</v>
       </c>
-      <c r="U35" t="n">
-        <v>0</v>
-      </c>
+      <c r="U35" t="inlineStr"/>
       <c r="V35" t="n">
         <v>8.050000000000001</v>
       </c>
-      <c r="W35" t="n">
-        <v>0</v>
-      </c>
+      <c r="W35" t="inlineStr"/>
       <c r="X35" t="n">
         <v>8.050000000000001</v>
       </c>
-      <c r="Y35" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA35" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y35" t="inlineStr"/>
+      <c r="Z35" t="inlineStr"/>
+      <c r="AA35" t="inlineStr"/>
       <c r="AB35" t="n">
         <v>11.53</v>
       </c>
-      <c r="AC35" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC35" t="inlineStr"/>
       <c r="AD35" t="n">
         <v>18</v>
       </c>
@@ -4814,84 +3794,58 @@
       <c r="D36" t="n">
         <v>8.23</v>
       </c>
-      <c r="E36" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" t="n">
-        <v>0</v>
-      </c>
-      <c r="G36" t="n">
-        <v>0</v>
-      </c>
-      <c r="H36" t="n">
-        <v>0</v>
-      </c>
+      <c r="E36" t="inlineStr"/>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
       <c r="I36" t="n">
         <v>12</v>
       </c>
       <c r="J36" t="n">
         <v>12.02</v>
       </c>
-      <c r="K36" t="n">
-        <v>0</v>
-      </c>
-      <c r="L36" t="n">
-        <v>0</v>
-      </c>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
       <c r="M36" t="n">
         <v>12</v>
       </c>
-      <c r="N36" t="n">
-        <v>0</v>
-      </c>
-      <c r="O36" t="n">
-        <v>0</v>
-      </c>
-      <c r="P36" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q36" t="n">
-        <v>0</v>
-      </c>
-      <c r="R36" t="n">
-        <v>0</v>
-      </c>
-      <c r="S36" t="n">
-        <v>0</v>
-      </c>
-      <c r="T36" t="n">
-        <v>0</v>
-      </c>
+      <c r="N36" t="inlineStr"/>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>UL</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr"/>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>UL</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr"/>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>UL</t>
+        </is>
+      </c>
+      <c r="T36" t="inlineStr"/>
       <c r="U36" t="n">
         <v>12</v>
       </c>
       <c r="V36" t="n">
         <v>12.08</v>
       </c>
-      <c r="W36" t="n">
-        <v>0</v>
-      </c>
-      <c r="X36" t="n">
-        <v>0</v>
-      </c>
+      <c r="W36" t="inlineStr"/>
+      <c r="X36" t="inlineStr"/>
       <c r="Y36" t="n">
         <v>12</v>
       </c>
       <c r="Z36" t="n">
         <v>12.43</v>
       </c>
-      <c r="AA36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD36" t="n">
-        <v>0</v>
-      </c>
+      <c r="AA36" t="inlineStr"/>
+      <c r="AB36" t="inlineStr"/>
+      <c r="AC36" t="inlineStr"/>
+      <c r="AD36" t="inlineStr"/>
       <c r="AE36" t="n">
         <v>8</v>
       </c>
@@ -4923,90 +3877,42 @@
           <t>ONEIDA CANAS CHICAS</t>
         </is>
       </c>
-      <c r="C37" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" t="n">
-        <v>0</v>
-      </c>
-      <c r="G37" t="n">
-        <v>0</v>
-      </c>
-      <c r="H37" t="n">
-        <v>0</v>
-      </c>
-      <c r="I37" t="n">
-        <v>0</v>
-      </c>
-      <c r="J37" t="n">
-        <v>0</v>
-      </c>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr"/>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
       <c r="K37" t="n">
         <v>3</v>
       </c>
       <c r="L37" t="n">
         <v>3.02</v>
       </c>
-      <c r="M37" t="n">
-        <v>0</v>
-      </c>
-      <c r="N37" t="n">
-        <v>0</v>
-      </c>
-      <c r="O37" t="n">
-        <v>0</v>
-      </c>
-      <c r="P37" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q37" t="n">
-        <v>0</v>
-      </c>
-      <c r="R37" t="n">
-        <v>0</v>
-      </c>
-      <c r="S37" t="n">
-        <v>0</v>
-      </c>
-      <c r="T37" t="n">
-        <v>0</v>
-      </c>
-      <c r="U37" t="n">
-        <v>0</v>
-      </c>
-      <c r="V37" t="n">
-        <v>0</v>
-      </c>
-      <c r="W37" t="n">
-        <v>0</v>
-      </c>
-      <c r="X37" t="n">
-        <v>0</v>
-      </c>
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr"/>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr"/>
+      <c r="R37" t="inlineStr"/>
+      <c r="S37" t="inlineStr"/>
+      <c r="T37" t="inlineStr"/>
+      <c r="U37" t="inlineStr"/>
+      <c r="V37" t="inlineStr"/>
+      <c r="W37" t="inlineStr"/>
+      <c r="X37" t="inlineStr"/>
       <c r="Y37" t="n">
         <v>3</v>
       </c>
       <c r="Z37" t="n">
         <v>3.35</v>
       </c>
-      <c r="AA37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD37" t="n">
-        <v>0</v>
-      </c>
+      <c r="AA37" t="inlineStr"/>
+      <c r="AB37" t="inlineStr"/>
+      <c r="AC37" t="inlineStr"/>
+      <c r="AD37" t="inlineStr"/>
       <c r="AE37" t="n">
         <v>0</v>
       </c>
@@ -5038,90 +3944,52 @@
           <t>Pragnya Tatikonda</t>
         </is>
       </c>
-      <c r="C38" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" t="n">
-        <v>0</v>
-      </c>
-      <c r="E38" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" t="n">
-        <v>0</v>
-      </c>
-      <c r="G38" t="n">
-        <v>0</v>
-      </c>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr"/>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
       <c r="H38" t="n">
         <v>6.6</v>
       </c>
-      <c r="I38" t="n">
-        <v>0</v>
-      </c>
+      <c r="I38" t="inlineStr"/>
       <c r="J38" t="n">
         <v>7.15</v>
       </c>
-      <c r="K38" t="n">
-        <v>0</v>
-      </c>
+      <c r="K38" t="inlineStr"/>
       <c r="L38" t="n">
         <v>5</v>
       </c>
-      <c r="M38" t="n">
-        <v>0</v>
-      </c>
+      <c r="M38" t="inlineStr"/>
       <c r="N38" t="n">
         <v>3.5</v>
       </c>
-      <c r="O38" t="n">
-        <v>0</v>
-      </c>
+      <c r="O38" t="inlineStr"/>
       <c r="P38" t="n">
         <v>5.6</v>
       </c>
-      <c r="Q38" t="n">
-        <v>0</v>
-      </c>
-      <c r="R38" t="n">
-        <v>0</v>
-      </c>
-      <c r="S38" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q38" t="inlineStr"/>
+      <c r="R38" t="inlineStr"/>
+      <c r="S38" t="inlineStr"/>
       <c r="T38" t="n">
         <v>6.35</v>
       </c>
-      <c r="U38" t="n">
-        <v>0</v>
-      </c>
+      <c r="U38" t="inlineStr"/>
       <c r="V38" t="n">
         <v>4.57</v>
       </c>
-      <c r="W38" t="n">
-        <v>0</v>
-      </c>
+      <c r="W38" t="inlineStr"/>
       <c r="X38" t="n">
         <v>4.27</v>
       </c>
-      <c r="Y38" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y38" t="inlineStr"/>
       <c r="Z38" t="n">
         <v>7</v>
       </c>
-      <c r="AA38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD38" t="n">
-        <v>0</v>
-      </c>
+      <c r="AA38" t="inlineStr"/>
+      <c r="AB38" t="inlineStr"/>
+      <c r="AC38" t="inlineStr"/>
+      <c r="AD38" t="inlineStr"/>
       <c r="AE38" t="n">
         <v>0</v>
       </c>
@@ -5153,24 +4021,16 @@
           <t>RONALD DESIR</t>
         </is>
       </c>
-      <c r="C39" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" t="n">
-        <v>0</v>
-      </c>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
       <c r="E39" t="n">
         <v>3</v>
       </c>
       <c r="F39" t="n">
         <v>3.38</v>
       </c>
-      <c r="G39" t="n">
-        <v>0</v>
-      </c>
-      <c r="H39" t="n">
-        <v>0</v>
-      </c>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
       <c r="I39" t="n">
         <v>3</v>
       </c>
@@ -5180,39 +4040,25 @@
       <c r="K39" t="n">
         <v>3</v>
       </c>
-      <c r="L39" t="n">
-        <v>0</v>
-      </c>
-      <c r="M39" t="n">
-        <v>0</v>
-      </c>
-      <c r="N39" t="n">
-        <v>0</v>
-      </c>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr"/>
       <c r="O39" t="n">
         <v>8</v>
       </c>
       <c r="P39" t="n">
         <v>8.35</v>
       </c>
-      <c r="Q39" t="n">
-        <v>0</v>
-      </c>
-      <c r="R39" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q39" t="inlineStr"/>
+      <c r="R39" t="inlineStr"/>
       <c r="S39" t="n">
         <v>3</v>
       </c>
       <c r="T39" t="n">
         <v>3.47</v>
       </c>
-      <c r="U39" t="n">
-        <v>0</v>
-      </c>
-      <c r="V39" t="n">
-        <v>0</v>
-      </c>
+      <c r="U39" t="inlineStr"/>
+      <c r="V39" t="inlineStr"/>
       <c r="W39" t="n">
         <v>3</v>
       </c>
@@ -5225,18 +4071,10 @@
       <c r="Z39" t="n">
         <v>3.17</v>
       </c>
-      <c r="AA39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD39" t="n">
-        <v>0</v>
-      </c>
+      <c r="AA39" t="inlineStr"/>
+      <c r="AB39" t="inlineStr"/>
+      <c r="AC39" t="inlineStr"/>
+      <c r="AD39" t="inlineStr"/>
       <c r="AE39" t="n">
         <v>0</v>
       </c>
@@ -5268,12 +4106,12 @@
           <t>Regine Salmon</t>
         </is>
       </c>
-      <c r="C40" t="n">
-        <v>0</v>
-      </c>
-      <c r="D40" t="n">
-        <v>0</v>
-      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>PTO</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr"/>
       <c r="E40" t="n">
         <v>12</v>
       </c>
@@ -5298,24 +4136,14 @@
       <c r="L40" t="n">
         <v>8.43</v>
       </c>
-      <c r="M40" t="n">
-        <v>0</v>
-      </c>
-      <c r="N40" t="n">
-        <v>0</v>
-      </c>
-      <c r="O40" t="n">
-        <v>0</v>
-      </c>
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr"/>
+      <c r="O40" t="inlineStr"/>
       <c r="P40" t="n">
         <v>1.98</v>
       </c>
-      <c r="Q40" t="n">
-        <v>0</v>
-      </c>
-      <c r="R40" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q40" t="inlineStr"/>
+      <c r="R40" t="inlineStr"/>
       <c r="S40" t="n">
         <v>12</v>
       </c>
@@ -5334,24 +4162,18 @@
       <c r="X40" t="n">
         <v>11.58</v>
       </c>
-      <c r="Y40" t="n">
-        <v>0</v>
+      <c r="Y40" t="inlineStr">
+        <is>
+          <t>PTO</t>
+        </is>
       </c>
       <c r="Z40" t="n">
         <v>8.369999999999999</v>
       </c>
-      <c r="AA40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD40" t="n">
-        <v>0</v>
-      </c>
+      <c r="AA40" t="inlineStr"/>
+      <c r="AB40" t="inlineStr"/>
+      <c r="AC40" t="inlineStr"/>
+      <c r="AD40" t="inlineStr"/>
       <c r="AE40" t="n">
         <v>0</v>
       </c>
@@ -5383,90 +4205,38 @@
           <t>SAMHITA GHORAKAVI</t>
         </is>
       </c>
-      <c r="C41" t="n">
-        <v>0</v>
-      </c>
-      <c r="D41" t="n">
-        <v>0</v>
-      </c>
-      <c r="E41" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" t="n">
-        <v>0</v>
-      </c>
-      <c r="G41" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" t="n">
-        <v>0</v>
-      </c>
-      <c r="I41" t="n">
-        <v>0</v>
-      </c>
-      <c r="J41" t="n">
-        <v>0</v>
-      </c>
-      <c r="K41" t="n">
-        <v>0</v>
-      </c>
-      <c r="L41" t="n">
-        <v>0</v>
-      </c>
-      <c r="M41" t="n">
-        <v>0</v>
-      </c>
-      <c r="N41" t="n">
-        <v>0</v>
-      </c>
-      <c r="O41" t="n">
-        <v>0</v>
-      </c>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr"/>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr"/>
       <c r="P41" t="n">
         <v>8.17</v>
       </c>
-      <c r="Q41" t="n">
-        <v>0</v>
-      </c>
-      <c r="R41" t="n">
-        <v>0</v>
-      </c>
-      <c r="S41" t="n">
-        <v>0</v>
-      </c>
-      <c r="T41" t="n">
-        <v>0</v>
-      </c>
-      <c r="U41" t="n">
-        <v>0</v>
-      </c>
-      <c r="V41" t="n">
-        <v>0</v>
-      </c>
-      <c r="W41" t="n">
-        <v>0</v>
-      </c>
-      <c r="X41" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y41" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB41" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q41" t="inlineStr"/>
+      <c r="R41" t="inlineStr"/>
+      <c r="S41" t="inlineStr"/>
+      <c r="T41" t="inlineStr"/>
+      <c r="U41" t="inlineStr"/>
+      <c r="V41" t="inlineStr"/>
+      <c r="W41" t="inlineStr"/>
+      <c r="X41" t="inlineStr"/>
+      <c r="Y41" t="inlineStr"/>
+      <c r="Z41" t="inlineStr"/>
+      <c r="AA41" t="inlineStr"/>
+      <c r="AB41" t="inlineStr"/>
       <c r="AC41" t="n">
         <v>8</v>
       </c>
-      <c r="AD41" t="n">
-        <v>0</v>
-      </c>
+      <c r="AD41" t="inlineStr"/>
       <c r="AE41" t="n">
         <v>0</v>
       </c>
@@ -5498,90 +4268,54 @@
           <t>SONIA GARCIA</t>
         </is>
       </c>
-      <c r="C42" t="n">
-        <v>0</v>
-      </c>
-      <c r="D42" t="n">
-        <v>0</v>
-      </c>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
       <c r="E42" t="n">
         <v>8.75</v>
       </c>
-      <c r="F42" t="n">
-        <v>0</v>
-      </c>
+      <c r="F42" t="inlineStr"/>
       <c r="G42" t="n">
         <v>8.75</v>
       </c>
-      <c r="H42" t="n">
-        <v>0</v>
-      </c>
+      <c r="H42" t="inlineStr"/>
       <c r="I42" t="n">
         <v>8.75</v>
       </c>
-      <c r="J42" t="n">
-        <v>0</v>
-      </c>
+      <c r="J42" t="inlineStr"/>
       <c r="K42" t="n">
         <v>8.75</v>
       </c>
-      <c r="L42" t="n">
-        <v>0</v>
-      </c>
+      <c r="L42" t="inlineStr"/>
       <c r="M42" t="n">
         <v>8.75</v>
       </c>
-      <c r="N42" t="n">
-        <v>0</v>
-      </c>
-      <c r="O42" t="n">
-        <v>0</v>
-      </c>
-      <c r="P42" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q42" t="n">
-        <v>0</v>
-      </c>
-      <c r="R42" t="n">
-        <v>0</v>
-      </c>
+      <c r="N42" t="inlineStr"/>
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr"/>
+      <c r="Q42" t="inlineStr"/>
+      <c r="R42" t="inlineStr"/>
       <c r="S42" t="n">
         <v>8.75</v>
       </c>
-      <c r="T42" t="n">
-        <v>0</v>
-      </c>
+      <c r="T42" t="inlineStr"/>
       <c r="U42" t="n">
         <v>8.75</v>
       </c>
-      <c r="V42" t="n">
-        <v>0</v>
-      </c>
+      <c r="V42" t="inlineStr"/>
       <c r="W42" t="n">
         <v>8.75</v>
       </c>
-      <c r="X42" t="n">
-        <v>0</v>
-      </c>
+      <c r="X42" t="inlineStr"/>
       <c r="Y42" t="n">
         <v>8.75</v>
       </c>
-      <c r="Z42" t="n">
-        <v>0</v>
-      </c>
+      <c r="Z42" t="inlineStr"/>
       <c r="AA42" t="n">
         <v>8.75</v>
       </c>
-      <c r="AB42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD42" t="n">
-        <v>0</v>
-      </c>
+      <c r="AB42" t="inlineStr"/>
+      <c r="AC42" t="inlineStr"/>
+      <c r="AD42" t="inlineStr"/>
       <c r="AE42" t="n">
         <v>0</v>
       </c>
@@ -5613,90 +4347,52 @@
           <t>Shivani Kapoor</t>
         </is>
       </c>
-      <c r="C43" t="n">
-        <v>0</v>
-      </c>
-      <c r="D43" t="n">
-        <v>0</v>
-      </c>
-      <c r="E43" t="n">
-        <v>0</v>
-      </c>
-      <c r="F43" t="n">
-        <v>0</v>
-      </c>
-      <c r="G43" t="n">
-        <v>0</v>
-      </c>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
       <c r="H43" t="n">
         <v>7.37</v>
       </c>
-      <c r="I43" t="n">
-        <v>0</v>
-      </c>
+      <c r="I43" t="inlineStr"/>
       <c r="J43" t="n">
         <v>7.7</v>
       </c>
-      <c r="K43" t="n">
-        <v>0</v>
-      </c>
+      <c r="K43" t="inlineStr"/>
       <c r="L43" t="n">
         <v>11.03</v>
       </c>
-      <c r="M43" t="n">
-        <v>0</v>
-      </c>
+      <c r="M43" t="inlineStr"/>
       <c r="N43" t="n">
         <v>6.67</v>
       </c>
-      <c r="O43" t="n">
-        <v>0</v>
-      </c>
+      <c r="O43" t="inlineStr"/>
       <c r="P43" t="n">
         <v>8.35</v>
       </c>
-      <c r="Q43" t="n">
-        <v>0</v>
-      </c>
-      <c r="R43" t="n">
-        <v>0</v>
-      </c>
-      <c r="S43" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q43" t="inlineStr"/>
+      <c r="R43" t="inlineStr"/>
+      <c r="S43" t="inlineStr"/>
       <c r="T43" t="n">
         <v>9.77</v>
       </c>
-      <c r="U43" t="n">
-        <v>0</v>
-      </c>
+      <c r="U43" t="inlineStr"/>
       <c r="V43" t="n">
         <v>6.23</v>
       </c>
-      <c r="W43" t="n">
-        <v>0</v>
-      </c>
+      <c r="W43" t="inlineStr"/>
       <c r="X43" t="n">
         <v>5.85</v>
       </c>
-      <c r="Y43" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y43" t="inlineStr"/>
       <c r="Z43" t="n">
         <v>9.43</v>
       </c>
-      <c r="AA43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD43" t="n">
-        <v>0</v>
-      </c>
+      <c r="AA43" t="inlineStr"/>
+      <c r="AB43" t="inlineStr"/>
+      <c r="AC43" t="inlineStr"/>
+      <c r="AD43" t="inlineStr"/>
       <c r="AE43" t="n">
         <v>0</v>
       </c>
@@ -5728,18 +4424,10 @@
           <t>TERRI STROBEL</t>
         </is>
       </c>
-      <c r="C44" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" t="n">
-        <v>0</v>
-      </c>
-      <c r="E44" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" t="n">
-        <v>0</v>
-      </c>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr"/>
+      <c r="F44" t="inlineStr"/>
       <c r="G44" t="n">
         <v>10</v>
       </c>
@@ -5764,24 +4452,12 @@
       <c r="N44" t="n">
         <v>13.7</v>
       </c>
-      <c r="O44" t="n">
-        <v>0</v>
-      </c>
-      <c r="P44" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q44" t="n">
-        <v>0</v>
-      </c>
-      <c r="R44" t="n">
-        <v>0</v>
-      </c>
-      <c r="S44" t="n">
-        <v>0</v>
-      </c>
-      <c r="T44" t="n">
-        <v>0</v>
-      </c>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr"/>
+      <c r="Q44" t="inlineStr"/>
+      <c r="R44" t="inlineStr"/>
+      <c r="S44" t="inlineStr"/>
+      <c r="T44" t="inlineStr"/>
       <c r="U44" t="n">
         <v>10</v>
       </c>
@@ -5791,9 +4467,7 @@
       <c r="W44" t="n">
         <v>10</v>
       </c>
-      <c r="X44" t="n">
-        <v>0</v>
-      </c>
+      <c r="X44" t="inlineStr"/>
       <c r="Y44" t="n">
         <v>10</v>
       </c>
@@ -5806,12 +4480,8 @@
       <c r="AB44" t="n">
         <v>12.78</v>
       </c>
-      <c r="AC44" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD44" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC44" t="inlineStr"/>
+      <c r="AD44" t="inlineStr"/>
       <c r="AE44" t="n">
         <v>0</v>
       </c>
@@ -5843,90 +4513,42 @@
           <t>Thomas Pearce</t>
         </is>
       </c>
-      <c r="C45" t="n">
-        <v>0</v>
-      </c>
-      <c r="D45" t="n">
-        <v>0</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" t="n">
-        <v>0</v>
-      </c>
-      <c r="G45" t="n">
-        <v>0</v>
-      </c>
-      <c r="H45" t="n">
-        <v>0</v>
-      </c>
-      <c r="I45" t="n">
-        <v>0</v>
-      </c>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr"/>
       <c r="J45" t="n">
         <v>2.73</v>
       </c>
-      <c r="K45" t="n">
-        <v>0</v>
-      </c>
-      <c r="L45" t="n">
-        <v>0</v>
-      </c>
-      <c r="M45" t="n">
-        <v>0</v>
-      </c>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
       <c r="N45" t="n">
         <v>2.7</v>
       </c>
-      <c r="O45" t="n">
-        <v>0</v>
-      </c>
-      <c r="P45" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q45" t="n">
-        <v>0</v>
-      </c>
-      <c r="R45" t="n">
-        <v>0</v>
-      </c>
-      <c r="S45" t="n">
-        <v>0</v>
-      </c>
-      <c r="T45" t="n">
-        <v>0</v>
-      </c>
-      <c r="U45" t="n">
-        <v>0</v>
-      </c>
-      <c r="V45" t="n">
-        <v>0</v>
-      </c>
-      <c r="W45" t="n">
-        <v>0</v>
-      </c>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
+      <c r="Q45" t="inlineStr"/>
+      <c r="R45" t="inlineStr"/>
+      <c r="S45" t="inlineStr"/>
+      <c r="T45" t="inlineStr"/>
+      <c r="U45" t="inlineStr"/>
+      <c r="V45" t="inlineStr"/>
+      <c r="W45" t="inlineStr"/>
       <c r="X45" t="n">
         <v>1.78</v>
       </c>
-      <c r="Y45" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA45" t="n">
-        <v>0</v>
-      </c>
+      <c r="Y45" t="inlineStr"/>
+      <c r="Z45" t="inlineStr"/>
+      <c r="AA45" t="inlineStr"/>
       <c r="AB45" t="n">
         <v>2.85</v>
       </c>
-      <c r="AC45" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD45" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC45" t="inlineStr"/>
+      <c r="AD45" t="inlineStr"/>
       <c r="AE45" t="n">
         <v>0</v>
       </c>
@@ -5958,12 +4580,8 @@
           <t>YOADAN ZEWDU</t>
         </is>
       </c>
-      <c r="C46" t="n">
-        <v>0</v>
-      </c>
-      <c r="D46" t="n">
-        <v>0</v>
-      </c>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
       <c r="E46" t="n">
         <v>9.25</v>
       </c>
@@ -5991,21 +4609,15 @@
       <c r="M46" t="n">
         <v>5.25</v>
       </c>
-      <c r="N46" t="n">
-        <v>0</v>
-      </c>
+      <c r="N46" t="inlineStr"/>
       <c r="O46" t="n">
         <v>8</v>
       </c>
       <c r="P46" t="n">
         <v>8.279999999999999</v>
       </c>
-      <c r="Q46" t="n">
-        <v>0</v>
-      </c>
-      <c r="R46" t="n">
-        <v>0</v>
-      </c>
+      <c r="Q46" t="inlineStr"/>
+      <c r="R46" t="inlineStr"/>
       <c r="S46" t="n">
         <v>9.25</v>
       </c>
@@ -6036,12 +4648,8 @@
       <c r="AB46" t="n">
         <v>4.87</v>
       </c>
-      <c r="AC46" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD46" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC46" t="inlineStr"/>
+      <c r="AD46" t="inlineStr"/>
       <c r="AE46" t="n">
         <v>0</v>
       </c>
@@ -6073,18 +4681,10 @@
           <t>ZO PARI BOCHUNG</t>
         </is>
       </c>
-      <c r="C47" t="n">
-        <v>0</v>
-      </c>
-      <c r="D47" t="n">
-        <v>0</v>
-      </c>
-      <c r="E47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" t="n">
-        <v>0</v>
-      </c>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr"/>
+      <c r="F47" t="inlineStr"/>
       <c r="G47" t="n">
         <v>10</v>
       </c>
@@ -6109,24 +4709,12 @@
       <c r="N47" t="n">
         <v>7.93</v>
       </c>
-      <c r="O47" t="n">
-        <v>0</v>
-      </c>
-      <c r="P47" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q47" t="n">
-        <v>0</v>
-      </c>
-      <c r="R47" t="n">
-        <v>0</v>
-      </c>
-      <c r="S47" t="n">
-        <v>0</v>
-      </c>
-      <c r="T47" t="n">
-        <v>0</v>
-      </c>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
+      <c r="Q47" t="inlineStr"/>
+      <c r="R47" t="inlineStr"/>
+      <c r="S47" t="inlineStr"/>
+      <c r="T47" t="inlineStr"/>
       <c r="U47" t="n">
         <v>10</v>
       </c>
@@ -6136,9 +4724,7 @@
       <c r="W47" t="n">
         <v>10</v>
       </c>
-      <c r="X47" t="n">
-        <v>0</v>
-      </c>
+      <c r="X47" t="inlineStr"/>
       <c r="Y47" t="n">
         <v>10</v>
       </c>
@@ -6151,12 +4737,8 @@
       <c r="AB47" t="n">
         <v>9.550000000000001</v>
       </c>
-      <c r="AC47" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD47" t="n">
-        <v>0</v>
-      </c>
+      <c r="AC47" t="inlineStr"/>
+      <c r="AD47" t="inlineStr"/>
       <c r="AE47" t="n">
         <v>0</v>
       </c>

</xml_diff>